<commit_message>
Fixed Test Report Generator path and updated Excel file
</commit_message>
<xml_diff>
--- a/TestReportGenerator/List of models.xlsx
+++ b/TestReportGenerator/List of models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Testing-app\TestReportGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505332D4-1AC3-418D-98E8-76A762B6F0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8384882-6F04-4B72-AB53-B65CDBE444B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
   <si>
     <t>MODEL</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>R80L</t>
+  </si>
+  <si>
+    <t>DS1250</t>
   </si>
 </sst>
 </file>
@@ -675,11 +678,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -893,17 +900,39 @@
       <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="C6" s="7">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7">
+        <v>415</v>
+      </c>
+      <c r="F6" s="7">
+        <v>50</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="7">
+        <v>2850</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="K6" s="8">
+        <v>26</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="M6" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">

</xml_diff>